<commit_message>
add html for different pages
</commit_message>
<xml_diff>
--- a/wireframes_4pages.xlsx
+++ b/wireframes_4pages.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emvan\GitHub_Repos\My_First_Multi_Page_Responsive_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9276EBE6-0549-4917-B713-7F31882E4E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA1D3D5-C670-4D6E-B556-9CF3BE1515B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-1160" windowWidth="25820" windowHeight="15500" xr2:uid="{AA3F40F2-1787-4AB6-A0CC-FF26B0CC094A}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
-    <sheet name="Play1" sheetId="2" r:id="rId2"/>
-    <sheet name="Play2" sheetId="3" r:id="rId3"/>
-    <sheet name="Play3" sheetId="4" r:id="rId4"/>
+    <sheet name="About" sheetId="5" r:id="rId2"/>
+    <sheet name="Play1-Logic" sheetId="2" r:id="rId3"/>
+    <sheet name="Play2-Play" sheetId="3" r:id="rId4"/>
+    <sheet name="Play3-Crafts" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="54">
   <si>
     <t>Logo</t>
   </si>
@@ -195,6 +196,12 @@
   </si>
   <si>
     <t>Arts &amp; Crafts 9</t>
+  </si>
+  <si>
+    <t>Play Ideas</t>
+  </si>
+  <si>
+    <t>About Creating As We Grow</t>
   </si>
 </sst>
 </file>
@@ -676,15 +683,15 @@
   <dimension ref="B2:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="12.36328125" customWidth="1"/>
+    <col min="1" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -692,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -707,8 +714,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -721,51 +728,51 @@
       <c r="K4" s="2"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -778,15 +785,15 @@
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -803,7 +810,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
@@ -817,7 +824,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="D18" s="5"/>
       <c r="F18" s="4"/>
@@ -825,7 +832,7 @@
       <c r="J18" s="4"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="D19" s="5"/>
       <c r="F19" s="4"/>
@@ -833,7 +840,7 @@
       <c r="J19" s="4"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="D20" s="5"/>
       <c r="F20" s="4"/>
@@ -841,7 +848,7 @@
       <c r="J20" s="4"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="D21" s="5"/>
       <c r="F21" s="4"/>
@@ -849,7 +856,7 @@
       <c r="J21" s="4"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="D22" s="5"/>
       <c r="F22" s="4"/>
@@ -857,7 +864,7 @@
       <c r="J22" s="4"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="10" t="s">
         <v>18</v>
@@ -874,7 +881,7 @@
       </c>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
@@ -885,8 +892,8 @@
       <c r="K24" s="7"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
@@ -902,7 +909,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="G27" s="5"/>
       <c r="I27" s="4" t="s">
@@ -910,25 +917,25 @@
       </c>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="G28" s="5"/>
       <c r="I28" s="4"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="G29" s="5"/>
       <c r="I29" s="4"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="G30" s="5"/>
       <c r="I30" s="4"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -938,11 +945,11 @@
       <c r="I31" s="4"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I32" s="4"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>22</v>
       </c>
@@ -954,31 +961,31 @@
       <c r="I33" s="4"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="G34" s="5"/>
       <c r="I34" s="4"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="G35" s="5"/>
       <c r="I35" s="4"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="G36" s="5"/>
       <c r="I36" s="4"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="G37" s="5"/>
       <c r="I37" s="4"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -990,7 +997,7 @@
       <c r="K38" s="7"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>10</v>
       </c>
@@ -1004,7 +1011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>23</v>
       </c>
@@ -1015,19 +1022,209 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6BB9B0-4B84-4B35-9191-C4CCF4E28D83}">
+  <dimension ref="B2:L42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="13" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1B74EF-A00F-4A71-823D-A1D850E92734}">
   <dimension ref="B2:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="12.36328125" customWidth="1"/>
+    <col min="1" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1050,8 +1247,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1068,7 +1265,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="D6" s="5"/>
       <c r="F6" s="4"/>
@@ -1076,7 +1273,7 @@
       <c r="J6" s="4"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="D7" s="5"/>
       <c r="F7" s="4"/>
@@ -1084,7 +1281,7 @@
       <c r="J7" s="4"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="D8" s="5"/>
       <c r="F8" s="4"/>
@@ -1092,7 +1289,7 @@
       <c r="J8" s="4"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="D9" s="5"/>
       <c r="F9" s="4"/>
@@ -1100,7 +1297,7 @@
       <c r="J9" s="4"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="D10" s="5"/>
       <c r="F10" s="4"/>
@@ -1108,7 +1305,7 @@
       <c r="J10" s="4"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="D11" s="5"/>
       <c r="F11" s="4"/>
@@ -1116,7 +1313,7 @@
       <c r="J11" s="4"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="10" t="s">
         <v>27</v>
@@ -1133,7 +1330,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
@@ -1144,8 +1341,8 @@
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1162,7 +1359,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="D16" s="5"/>
       <c r="F16" s="4"/>
@@ -1170,7 +1367,7 @@
       <c r="J16" s="4"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="D17" s="5"/>
       <c r="F17" s="4"/>
@@ -1178,7 +1375,7 @@
       <c r="J17" s="4"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="D18" s="5"/>
       <c r="F18" s="4"/>
@@ -1186,7 +1383,7 @@
       <c r="J18" s="4"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="D19" s="5"/>
       <c r="F19" s="4"/>
@@ -1194,7 +1391,7 @@
       <c r="J19" s="4"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="D20" s="5"/>
       <c r="F20" s="4"/>
@@ -1202,7 +1399,7 @@
       <c r="J20" s="4"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="D21" s="5"/>
       <c r="F21" s="4"/>
@@ -1210,7 +1407,7 @@
       <c r="J21" s="4"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="10" t="s">
         <v>27</v>
@@ -1227,7 +1424,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
@@ -1238,8 +1435,8 @@
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1256,7 +1453,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="D26" s="5"/>
       <c r="F26" s="4"/>
@@ -1264,7 +1461,7 @@
       <c r="J26" s="4"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="D27" s="5"/>
       <c r="F27" s="4"/>
@@ -1272,7 +1469,7 @@
       <c r="J27" s="4"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="D28" s="5"/>
       <c r="F28" s="4"/>
@@ -1280,7 +1477,7 @@
       <c r="J28" s="4"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="D29" s="5"/>
       <c r="F29" s="4"/>
@@ -1288,7 +1485,7 @@
       <c r="J29" s="4"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4"/>
@@ -1296,7 +1493,7 @@
       <c r="J30" s="4"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="D31" s="5"/>
       <c r="F31" s="4"/>
@@ -1304,7 +1501,7 @@
       <c r="J31" s="4"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="10" t="s">
         <v>27</v>
@@ -1321,7 +1518,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
@@ -1332,7 +1529,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>10</v>
       </c>
@@ -1346,7 +1543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>23</v>
       </c>
@@ -1356,7 +1553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C355D5B-B475-49FC-AED6-7E9FC4155F75}">
   <dimension ref="B2:L42"/>
   <sheetViews>
@@ -1364,12 +1561,12 @@
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="12.36328125" customWidth="1"/>
+    <col min="1" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1392,8 +1589,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1410,7 +1607,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="D6" s="5"/>
       <c r="F6" s="4"/>
@@ -1418,7 +1615,7 @@
       <c r="J6" s="4"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="D7" s="5"/>
       <c r="F7" s="4"/>
@@ -1426,7 +1623,7 @@
       <c r="J7" s="4"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="D8" s="5"/>
       <c r="F8" s="4"/>
@@ -1434,7 +1631,7 @@
       <c r="J8" s="4"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="D9" s="5"/>
       <c r="F9" s="4"/>
@@ -1442,7 +1639,7 @@
       <c r="J9" s="4"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="D10" s="5"/>
       <c r="F10" s="4"/>
@@ -1450,7 +1647,7 @@
       <c r="J10" s="4"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="D11" s="5"/>
       <c r="F11" s="4"/>
@@ -1458,7 +1655,7 @@
       <c r="J11" s="4"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="10" t="s">
         <v>27</v>
@@ -1475,7 +1672,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
@@ -1486,8 +1683,8 @@
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1504,7 +1701,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="D16" s="5"/>
       <c r="F16" s="4"/>
@@ -1512,7 +1709,7 @@
       <c r="J16" s="4"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="D17" s="5"/>
       <c r="F17" s="4"/>
@@ -1520,7 +1717,7 @@
       <c r="J17" s="4"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="D18" s="5"/>
       <c r="F18" s="4"/>
@@ -1528,7 +1725,7 @@
       <c r="J18" s="4"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="D19" s="5"/>
       <c r="F19" s="4"/>
@@ -1536,7 +1733,7 @@
       <c r="J19" s="4"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="D20" s="5"/>
       <c r="F20" s="4"/>
@@ -1544,7 +1741,7 @@
       <c r="J20" s="4"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="D21" s="5"/>
       <c r="F21" s="4"/>
@@ -1552,7 +1749,7 @@
       <c r="J21" s="4"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="10" t="s">
         <v>27</v>
@@ -1569,7 +1766,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
@@ -1580,8 +1777,8 @@
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>40</v>
       </c>
@@ -1598,7 +1795,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="D26" s="5"/>
       <c r="F26" s="4"/>
@@ -1606,7 +1803,7 @@
       <c r="J26" s="4"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="D27" s="5"/>
       <c r="F27" s="4"/>
@@ -1614,7 +1811,7 @@
       <c r="J27" s="4"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="D28" s="5"/>
       <c r="F28" s="4"/>
@@ -1622,7 +1819,7 @@
       <c r="J28" s="4"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="D29" s="5"/>
       <c r="F29" s="4"/>
@@ -1630,7 +1827,7 @@
       <c r="J29" s="4"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4"/>
@@ -1638,7 +1835,7 @@
       <c r="J30" s="4"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="D31" s="5"/>
       <c r="F31" s="4"/>
@@ -1646,7 +1843,7 @@
       <c r="J31" s="4"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="10" t="s">
         <v>27</v>
@@ -1663,7 +1860,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
@@ -1674,7 +1871,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>10</v>
       </c>
@@ -1688,7 +1885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>23</v>
       </c>
@@ -1698,20 +1895,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2746FE12-8835-41BF-A80C-B8A3B40DC7FC}">
   <dimension ref="B2:L42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="12.36328125" customWidth="1"/>
+    <col min="1" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1734,8 +1931,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1752,7 +1949,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="D6" s="5"/>
       <c r="F6" s="4"/>
@@ -1760,7 +1957,7 @@
       <c r="J6" s="4"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="D7" s="5"/>
       <c r="F7" s="4"/>
@@ -1768,7 +1965,7 @@
       <c r="J7" s="4"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="D8" s="5"/>
       <c r="F8" s="4"/>
@@ -1776,7 +1973,7 @@
       <c r="J8" s="4"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="D9" s="5"/>
       <c r="F9" s="4"/>
@@ -1784,7 +1981,7 @@
       <c r="J9" s="4"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="D10" s="5"/>
       <c r="F10" s="4"/>
@@ -1792,7 +1989,7 @@
       <c r="J10" s="4"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="D11" s="5"/>
       <c r="F11" s="4"/>
@@ -1800,7 +1997,7 @@
       <c r="J11" s="4"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="10" t="s">
         <v>27</v>
@@ -1817,7 +2014,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
@@ -1828,8 +2025,8 @@
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
@@ -1846,7 +2043,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="D16" s="5"/>
       <c r="F16" s="4"/>
@@ -1854,7 +2051,7 @@
       <c r="J16" s="4"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="D17" s="5"/>
       <c r="F17" s="4"/>
@@ -1862,7 +2059,7 @@
       <c r="J17" s="4"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="D18" s="5"/>
       <c r="F18" s="4"/>
@@ -1870,7 +2067,7 @@
       <c r="J18" s="4"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="D19" s="5"/>
       <c r="F19" s="4"/>
@@ -1878,7 +2075,7 @@
       <c r="J19" s="4"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="D20" s="5"/>
       <c r="F20" s="4"/>
@@ -1886,7 +2083,7 @@
       <c r="J20" s="4"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="D21" s="5"/>
       <c r="F21" s="4"/>
@@ -1894,7 +2091,7 @@
       <c r="J21" s="4"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="10" t="s">
         <v>27</v>
@@ -1911,7 +2108,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
@@ -1922,8 +2119,8 @@
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1940,7 +2137,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="D26" s="5"/>
       <c r="F26" s="4"/>
@@ -1948,7 +2145,7 @@
       <c r="J26" s="4"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="D27" s="5"/>
       <c r="F27" s="4"/>
@@ -1956,7 +2153,7 @@
       <c r="J27" s="4"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="D28" s="5"/>
       <c r="F28" s="4"/>
@@ -1964,7 +2161,7 @@
       <c r="J28" s="4"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="D29" s="5"/>
       <c r="F29" s="4"/>
@@ -1972,7 +2169,7 @@
       <c r="J29" s="4"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4"/>
@@ -1980,7 +2177,7 @@
       <c r="J30" s="4"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="D31" s="5"/>
       <c r="F31" s="4"/>
@@ -1988,7 +2185,7 @@
       <c r="J31" s="4"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="10" t="s">
         <v>27</v>
@@ -2005,7 +2202,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
@@ -2016,7 +2213,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>10</v>
       </c>
@@ -2030,7 +2227,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>23</v>
       </c>

</xml_diff>